<commit_message>
ng: update bauchi forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2024/bauchi/nov 2024/ng_oncho_2411_1_community_bau.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2024/bauchi/nov 2024/ng_oncho_2411_1_community_bau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\bauchi\nov 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D8B24-BFFF-463A-8F2F-6C15E8E5AFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD335D7-E15B-499B-856A-DA3F1EC2B846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="182">
   <si>
     <t>type</t>
   </si>
@@ -392,12 +392,6 @@
     <t>lga = ${r_lga}</t>
   </si>
   <si>
-    <t>ng_oncho_2026_1_com_bau</t>
-  </si>
-  <si>
-    <t>(Bauchi) 1. Community Registration Form</t>
-  </si>
-  <si>
     <t>BAU_ALK_N_001</t>
   </si>
   <si>
@@ -507,6 +501,87 @@
   </si>
   <si>
     <t>site_id</t>
+  </si>
+  <si>
+    <t>ng_oncho_2411_1_community_bau_v2</t>
+  </si>
+  <si>
+    <t>(Bauchi) 1. Community Registration Form V2</t>
+  </si>
+  <si>
+    <t>ITAS/GADAU</t>
+  </si>
+  <si>
+    <t>KATAGUM</t>
+  </si>
+  <si>
+    <t>JAMA ARE</t>
+  </si>
+  <si>
+    <t>KAFIN MADAKI</t>
+  </si>
+  <si>
+    <t>SABON GARIN YAMRAT</t>
+  </si>
+  <si>
+    <t>BAKIN KANAKA</t>
+  </si>
+  <si>
+    <t>WAILO</t>
+  </si>
+  <si>
+    <t>ZUBUKI</t>
+  </si>
+  <si>
+    <t>GONGO</t>
+  </si>
+  <si>
+    <t>YAYU</t>
+  </si>
+  <si>
+    <t>GAKA</t>
+  </si>
+  <si>
+    <t>KAWARI</t>
+  </si>
+  <si>
+    <t>BAKIN KOGI</t>
+  </si>
+  <si>
+    <t>BAUSHE ILA</t>
+  </si>
+  <si>
+    <t>BAU_ALK_G_037</t>
+  </si>
+  <si>
+    <t>BAU_TOR_G_038</t>
+  </si>
+  <si>
+    <t>BAU_KIR_E_039</t>
+  </si>
+  <si>
+    <t>BAU_TOR_G_040</t>
+  </si>
+  <si>
+    <t>BAU_BAU_G_041</t>
+  </si>
+  <si>
+    <t>BAU_GAN_G_042</t>
+  </si>
+  <si>
+    <t>BAU_GAN_G_043</t>
+  </si>
+  <si>
+    <t>BAU_NIN_G_044</t>
+  </si>
+  <si>
+    <t>BAU_JAM_G_045</t>
+  </si>
+  <si>
+    <t>BAU_ITA_G_046</t>
+  </si>
+  <si>
+    <t>BAU_KAT_G_047</t>
   </si>
 </sst>
 </file>
@@ -1413,11 +1488,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1594,10 +1669,10 @@
         <v>108</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>54</v>
@@ -1608,10 +1683,10 @@
         <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
         <v>54</v>
@@ -1622,10 +1697,10 @@
         <v>108</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
         <v>54</v>
@@ -1636,10 +1711,10 @@
         <v>108</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
@@ -1650,10 +1725,10 @@
         <v>108</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>54</v>
@@ -1664,10 +1739,10 @@
         <v>108</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -1678,10 +1753,10 @@
         <v>108</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>54</v>
@@ -1692,10 +1767,10 @@
         <v>108</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
@@ -1706,66 +1781,69 @@
         <v>108</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>54</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>113</v>
+      <c r="A25" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>113</v>
+      <c r="A26" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
+      <c r="A27" s="23"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>113</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
         <v>55</v>
@@ -1776,13 +1854,13 @@
         <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,13 +1868,13 @@
         <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,13 +1882,13 @@
         <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1818,13 +1896,13 @@
         <v>113</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1832,13 +1910,13 @@
         <v>113</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1846,27 +1924,27 @@
         <v>113</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>113</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,13 +1952,13 @@
         <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,13 +1966,13 @@
         <v>113</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,13 +1980,13 @@
         <v>113</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,13 +1994,13 @@
         <v>113</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1930,13 +2008,13 @@
         <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1944,13 +2022,13 @@
         <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1958,13 +2036,13 @@
         <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,13 +2050,13 @@
         <v>113</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1986,13 +2064,13 @@
         <v>113</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2000,13 +2078,13 @@
         <v>113</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="E45" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,13 +2092,13 @@
         <v>113</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2028,13 +2106,13 @@
         <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2042,685 +2120,1035 @@
         <v>113</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>113</v>
-      </c>
-      <c r="B49" s="1" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E61" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50" s="1" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="1" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E63" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="1" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E64" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="1" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="1" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" s="1" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="1" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E70" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>113</v>
-      </c>
-      <c r="B57" s="1" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E71" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="1" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="1" t="s">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E73" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="1" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E74" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F62" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F64" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F65" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F67" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F68" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F69" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F70" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F71" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F72" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F74" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F75" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="F76" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F77" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="F78" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F79" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F80" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F81" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F82" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="F83" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F84" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F85" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F86" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F87" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="F88" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F89" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F90" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="F91" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F92" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="F93" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="F94" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F95" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="F96" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="F97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F98" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F101" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F102" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F104" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F105" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F106" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F107" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F108" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F110" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F111" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F112" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F113" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F114" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F115" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F116" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F118" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F119" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F120" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F121" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F122" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2733,7 +3161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2758,10 +3186,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>

</xml_diff>